<commit_message>
30.12.2020 MC Sales Deails
</commit_message>
<xml_diff>
--- a/2020/December/All Details/12.12.2020/MC Bank Statement Dec-2020.xlsx
+++ b/2020/December/All Details/12.12.2020/MC Bank Statement Dec-2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 2020" sheetId="7" r:id="rId1"/>
@@ -2819,12 +2819,36 @@
     <xf numFmtId="2" fontId="41" fillId="43" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="39" fillId="44" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="44" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2852,12 +2876,6 @@
     <xf numFmtId="1" fontId="39" fillId="35" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2870,18 +2888,6 @@
     <xf numFmtId="0" fontId="39" fillId="35" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="39" fillId="35" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2953,12 +2959,6 @@
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="44" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="44" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="55">
@@ -3051,7 +3051,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3063,7 +3063,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3086,14 +3086,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3181,7 +3181,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3193,7 +3193,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3216,14 +3216,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3255,7 +3255,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3267,7 +3267,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3290,14 +3290,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3623,21 +3623,21 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="20.25">
-      <c r="B2" s="283" t="s">
+      <c r="B2" s="285" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="283"/>
-      <c r="D2" s="283"/>
-      <c r="E2" s="283"/>
+      <c r="C2" s="285"/>
+      <c r="D2" s="285"/>
+      <c r="E2" s="285"/>
     </row>
     <row r="3" spans="1:8" ht="16.5" customHeight="1">
       <c r="A3" s="35"/>
-      <c r="B3" s="284" t="s">
+      <c r="B3" s="286" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="284"/>
-      <c r="D3" s="284"/>
-      <c r="E3" s="284"/>
+      <c r="C3" s="286"/>
+      <c r="D3" s="286"/>
+      <c r="E3" s="286"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="B4" s="36" t="s">
@@ -4723,73 +4723,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25">
-      <c r="A1" s="285" t="s">
+      <c r="A1" s="293" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="285"/>
-      <c r="C1" s="285"/>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
-      <c r="H1" s="285"/>
-      <c r="I1" s="285"/>
-      <c r="J1" s="285"/>
-      <c r="K1" s="285"/>
-      <c r="L1" s="285"/>
-      <c r="M1" s="285"/>
-      <c r="N1" s="285"/>
-      <c r="O1" s="285"/>
-      <c r="P1" s="285"/>
-      <c r="Q1" s="285"/>
-      <c r="R1" s="285"/>
-      <c r="S1" s="285"/>
+      <c r="B1" s="293"/>
+      <c r="C1" s="293"/>
+      <c r="D1" s="293"/>
+      <c r="E1" s="293"/>
+      <c r="F1" s="293"/>
+      <c r="G1" s="293"/>
+      <c r="H1" s="293"/>
+      <c r="I1" s="293"/>
+      <c r="J1" s="293"/>
+      <c r="K1" s="293"/>
+      <c r="L1" s="293"/>
+      <c r="M1" s="293"/>
+      <c r="N1" s="293"/>
+      <c r="O1" s="293"/>
+      <c r="P1" s="293"/>
+      <c r="Q1" s="293"/>
+      <c r="R1" s="293"/>
+      <c r="S1" s="293"/>
     </row>
     <row r="2" spans="1:26" s="203" customFormat="1" ht="18">
-      <c r="A2" s="286" t="s">
+      <c r="A2" s="294" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="286"/>
-      <c r="C2" s="286"/>
-      <c r="D2" s="286"/>
-      <c r="E2" s="286"/>
-      <c r="F2" s="286"/>
-      <c r="G2" s="286"/>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
-      <c r="K2" s="286"/>
-      <c r="L2" s="286"/>
-      <c r="M2" s="286"/>
-      <c r="N2" s="286"/>
-      <c r="O2" s="286"/>
-      <c r="P2" s="286"/>
-      <c r="Q2" s="286"/>
-      <c r="R2" s="286"/>
-      <c r="S2" s="286"/>
+      <c r="B2" s="294"/>
+      <c r="C2" s="294"/>
+      <c r="D2" s="294"/>
+      <c r="E2" s="294"/>
+      <c r="F2" s="294"/>
+      <c r="G2" s="294"/>
+      <c r="H2" s="294"/>
+      <c r="I2" s="294"/>
+      <c r="J2" s="294"/>
+      <c r="K2" s="294"/>
+      <c r="L2" s="294"/>
+      <c r="M2" s="294"/>
+      <c r="N2" s="294"/>
+      <c r="O2" s="294"/>
+      <c r="P2" s="294"/>
+      <c r="Q2" s="294"/>
+      <c r="R2" s="294"/>
+      <c r="S2" s="294"/>
     </row>
     <row r="3" spans="1:26" s="204" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A3" s="287" t="s">
+      <c r="A3" s="295" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="288"/>
-      <c r="C3" s="288"/>
-      <c r="D3" s="288"/>
-      <c r="E3" s="288"/>
-      <c r="F3" s="288"/>
-      <c r="G3" s="288"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="288"/>
-      <c r="J3" s="288"/>
-      <c r="K3" s="288"/>
-      <c r="L3" s="288"/>
-      <c r="M3" s="288"/>
-      <c r="N3" s="288"/>
-      <c r="O3" s="288"/>
-      <c r="P3" s="288"/>
-      <c r="Q3" s="288"/>
-      <c r="R3" s="288"/>
-      <c r="S3" s="289"/>
+      <c r="B3" s="296"/>
+      <c r="C3" s="296"/>
+      <c r="D3" s="296"/>
+      <c r="E3" s="296"/>
+      <c r="F3" s="296"/>
+      <c r="G3" s="296"/>
+      <c r="H3" s="296"/>
+      <c r="I3" s="296"/>
+      <c r="J3" s="296"/>
+      <c r="K3" s="296"/>
+      <c r="L3" s="296"/>
+      <c r="M3" s="296"/>
+      <c r="N3" s="296"/>
+      <c r="O3" s="296"/>
+      <c r="P3" s="296"/>
+      <c r="Q3" s="296"/>
+      <c r="R3" s="296"/>
+      <c r="S3" s="297"/>
       <c r="U3" s="116"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
@@ -4798,58 +4798,58 @@
       <c r="Z3" s="29"/>
     </row>
     <row r="4" spans="1:26" s="206" customFormat="1">
-      <c r="A4" s="290" t="s">
+      <c r="A4" s="298" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="292" t="s">
+      <c r="B4" s="300" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="294" t="s">
+      <c r="C4" s="287" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="294" t="s">
+      <c r="D4" s="287" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="294" t="s">
+      <c r="E4" s="287" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="294" t="s">
+      <c r="F4" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="294" t="s">
+      <c r="G4" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="294" t="s">
+      <c r="H4" s="287" t="s">
         <v>107</v>
       </c>
-      <c r="I4" s="294" t="s">
+      <c r="I4" s="287" t="s">
         <v>133</v>
       </c>
-      <c r="J4" s="294" t="s">
+      <c r="J4" s="287" t="s">
         <v>108</v>
       </c>
-      <c r="K4" s="294" t="s">
+      <c r="K4" s="287" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="294" t="s">
+      <c r="L4" s="287" t="s">
         <v>110</v>
       </c>
-      <c r="M4" s="294" t="s">
+      <c r="M4" s="287" t="s">
         <v>111</v>
       </c>
-      <c r="N4" s="294" t="s">
+      <c r="N4" s="287" t="s">
         <v>112</v>
       </c>
-      <c r="O4" s="300" t="s">
+      <c r="O4" s="289" t="s">
         <v>113</v>
       </c>
-      <c r="P4" s="302" t="s">
+      <c r="P4" s="291" t="s">
         <v>114</v>
       </c>
-      <c r="Q4" s="298" t="s">
+      <c r="Q4" s="304" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="296" t="s">
+      <c r="R4" s="302" t="s">
         <v>115</v>
       </c>
       <c r="S4" s="205" t="s">
@@ -4862,24 +4862,24 @@
       <c r="Y4" s="208"/>
     </row>
     <row r="5" spans="1:26" s="206" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A5" s="291"/>
-      <c r="B5" s="293"/>
-      <c r="C5" s="295"/>
-      <c r="D5" s="295"/>
-      <c r="E5" s="295"/>
-      <c r="F5" s="295"/>
-      <c r="G5" s="295"/>
-      <c r="H5" s="295"/>
-      <c r="I5" s="295"/>
-      <c r="J5" s="295"/>
-      <c r="K5" s="295"/>
-      <c r="L5" s="295"/>
-      <c r="M5" s="295"/>
-      <c r="N5" s="295"/>
-      <c r="O5" s="301"/>
-      <c r="P5" s="303"/>
-      <c r="Q5" s="299"/>
-      <c r="R5" s="297"/>
+      <c r="A5" s="299"/>
+      <c r="B5" s="301"/>
+      <c r="C5" s="288"/>
+      <c r="D5" s="288"/>
+      <c r="E5" s="288"/>
+      <c r="F5" s="288"/>
+      <c r="G5" s="288"/>
+      <c r="H5" s="288"/>
+      <c r="I5" s="288"/>
+      <c r="J5" s="288"/>
+      <c r="K5" s="288"/>
+      <c r="L5" s="288"/>
+      <c r="M5" s="288"/>
+      <c r="N5" s="288"/>
+      <c r="O5" s="290"/>
+      <c r="P5" s="292"/>
+      <c r="Q5" s="305"/>
+      <c r="R5" s="303"/>
       <c r="S5" s="210" t="s">
         <v>116</v>
       </c>
@@ -7998,11 +7998,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -8019,6 +8014,11 @@
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8031,8 +8031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI246"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -8058,14 +8058,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61" ht="19.5">
-      <c r="A1" s="310" t="s">
+      <c r="A1" s="312" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="310"/>
-      <c r="C1" s="310"/>
-      <c r="D1" s="310"/>
-      <c r="E1" s="310"/>
-      <c r="F1" s="310"/>
+      <c r="B1" s="312"/>
+      <c r="C1" s="312"/>
+      <c r="D1" s="312"/>
+      <c r="E1" s="312"/>
+      <c r="F1" s="312"/>
       <c r="L1" s="102"/>
       <c r="M1" s="262"/>
       <c r="N1" s="262"/>
@@ -8118,14 +8118,14 @@
       <c r="BI1" s="262"/>
     </row>
     <row r="2" spans="1:61" ht="15">
-      <c r="A2" s="311" t="s">
+      <c r="A2" s="313" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="311"/>
-      <c r="C2" s="311"/>
-      <c r="D2" s="311"/>
-      <c r="E2" s="311"/>
-      <c r="F2" s="311"/>
+      <c r="B2" s="313"/>
+      <c r="C2" s="313"/>
+      <c r="D2" s="313"/>
+      <c r="E2" s="313"/>
+      <c r="F2" s="313"/>
       <c r="L2" s="102"/>
       <c r="M2" s="262"/>
       <c r="N2" s="262"/>
@@ -8178,14 +8178,14 @@
       <c r="BI2" s="262"/>
     </row>
     <row r="3" spans="1:61">
-      <c r="A3" s="312" t="s">
+      <c r="A3" s="314" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="312"/>
-      <c r="C3" s="312"/>
-      <c r="D3" s="312"/>
-      <c r="E3" s="312"/>
-      <c r="F3" s="312"/>
+      <c r="B3" s="314"/>
+      <c r="C3" s="314"/>
+      <c r="D3" s="314"/>
+      <c r="E3" s="314"/>
+      <c r="F3" s="314"/>
       <c r="K3" s="262"/>
       <c r="L3" s="102"/>
       <c r="M3" s="262"/>
@@ -10449,12 +10449,12 @@
       <c r="BI34" s="262"/>
     </row>
     <row r="35" spans="1:61" ht="13.5" thickBot="1">
-      <c r="A35" s="313" t="s">
+      <c r="A35" s="315" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="314"/>
-      <c r="C35" s="314"/>
-      <c r="D35" s="315"/>
+      <c r="B35" s="316"/>
+      <c r="C35" s="316"/>
+      <c r="D35" s="317"/>
       <c r="E35" s="116"/>
       <c r="F35" s="118"/>
       <c r="G35" s="132"/>
@@ -11021,13 +11021,13 @@
       <c r="C43" s="110"/>
       <c r="D43" s="142"/>
       <c r="E43" s="116"/>
-      <c r="F43" s="316" t="s">
+      <c r="F43" s="318" t="s">
         <v>54</v>
       </c>
-      <c r="G43" s="316"/>
-      <c r="H43" s="316"/>
-      <c r="I43" s="316"/>
-      <c r="J43" s="316"/>
+      <c r="G43" s="318"/>
+      <c r="H43" s="318"/>
+      <c r="I43" s="318"/>
+      <c r="J43" s="318"/>
       <c r="K43" s="149"/>
       <c r="L43" s="107"/>
       <c r="M43" s="262"/>
@@ -11215,7 +11215,7 @@
         <v>27</v>
       </c>
       <c r="B46" s="153"/>
-      <c r="C46" s="329">
+      <c r="C46" s="284">
         <v>14450</v>
       </c>
       <c r="D46" s="154" t="s">
@@ -11555,7 +11555,7 @@
         <v>55</v>
       </c>
       <c r="B51" s="107"/>
-      <c r="C51" s="328">
+      <c r="C51" s="283">
         <v>85435</v>
       </c>
       <c r="D51" s="160" t="s">
@@ -12286,17 +12286,17 @@
       <c r="BI61" s="262"/>
     </row>
     <row r="62" spans="1:61">
-      <c r="A62" s="317" t="s">
+      <c r="A62" s="319" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="318"/>
+      <c r="B62" s="320"/>
       <c r="C62" s="156"/>
       <c r="D62" s="163"/>
       <c r="E62" s="124"/>
-      <c r="F62" s="304" t="s">
+      <c r="F62" s="306" t="s">
         <v>167</v>
       </c>
-      <c r="G62" s="304"/>
+      <c r="G62" s="306"/>
       <c r="H62" s="261"/>
       <c r="I62" s="261"/>
       <c r="J62" s="164" t="s">
@@ -13091,7 +13091,7 @@
         <v>79</v>
       </c>
       <c r="B72" s="107"/>
-      <c r="C72" s="328">
+      <c r="C72" s="283">
         <v>3500</v>
       </c>
       <c r="D72" s="160" t="s">
@@ -13171,7 +13171,7 @@
         <v>81</v>
       </c>
       <c r="B73" s="107"/>
-      <c r="C73" s="328">
+      <c r="C73" s="283">
         <v>14560</v>
       </c>
       <c r="D73" s="160" t="s">
@@ -13651,7 +13651,7 @@
         <v>88</v>
       </c>
       <c r="B79" s="107"/>
-      <c r="C79" s="328">
+      <c r="C79" s="283">
         <v>5000</v>
       </c>
       <c r="D79" s="160" t="s">
@@ -14131,7 +14131,7 @@
         <v>36</v>
       </c>
       <c r="B85" s="107"/>
-      <c r="C85" s="328">
+      <c r="C85" s="283">
         <v>129725</v>
       </c>
       <c r="D85" s="160" t="s">
@@ -15696,7 +15696,7 @@
       <c r="B105" s="178" t="s">
         <v>61</v>
       </c>
-      <c r="C105" s="328">
+      <c r="C105" s="283">
         <v>2340</v>
       </c>
       <c r="D105" s="157" t="s">
@@ -15856,7 +15856,7 @@
       <c r="B107" s="157">
         <v>1763999686</v>
       </c>
-      <c r="C107" s="328">
+      <c r="C107" s="283">
         <v>5340</v>
       </c>
       <c r="D107" s="157" t="s">
@@ -15937,7 +15937,7 @@
       <c r="B108" s="107" t="s">
         <v>52</v>
       </c>
-      <c r="C108" s="328">
+      <c r="C108" s="283">
         <v>1190</v>
       </c>
       <c r="D108" s="160" t="s">
@@ -16018,7 +16018,7 @@
       <c r="B109" s="157">
         <v>1758900692</v>
       </c>
-      <c r="C109" s="328">
+      <c r="C109" s="283">
         <v>30000</v>
       </c>
       <c r="D109" s="157" t="s">
@@ -16101,7 +16101,7 @@
       <c r="B110" s="157" t="s">
         <v>61</v>
       </c>
-      <c r="C110" s="328">
+      <c r="C110" s="283">
         <v>6300</v>
       </c>
       <c r="D110" s="157" t="s">
@@ -16338,10 +16338,10 @@
       <c r="BI112" s="262"/>
     </row>
     <row r="113" spans="1:61">
-      <c r="A113" s="305" t="s">
+      <c r="A113" s="307" t="s">
         <v>97</v>
       </c>
-      <c r="B113" s="306"/>
+      <c r="B113" s="308"/>
       <c r="C113" s="179">
         <f>SUM(C37:C112)</f>
         <v>2397722</v>
@@ -16491,10 +16491,10 @@
       <c r="BI114" s="262"/>
     </row>
     <row r="115" spans="1:61">
-      <c r="A115" s="307" t="s">
+      <c r="A115" s="309" t="s">
         <v>98</v>
       </c>
-      <c r="B115" s="308"/>
+      <c r="B115" s="310"/>
       <c r="C115" s="184">
         <f>C113+L136</f>
         <v>2397722</v>
@@ -18469,8 +18469,8 @@
       <c r="N169" s="266"/>
     </row>
     <row r="170" spans="5:14">
-      <c r="F170" s="309"/>
-      <c r="G170" s="309"/>
+      <c r="F170" s="311"/>
+      <c r="G170" s="311"/>
       <c r="H170" s="262"/>
       <c r="I170" s="122"/>
       <c r="J170" s="102"/>
@@ -19129,7 +19129,7 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -19148,24 +19148,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="26.25">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="321" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="320"/>
-      <c r="C1" s="320"/>
-      <c r="D1" s="320"/>
-      <c r="E1" s="321"/>
+      <c r="B1" s="322"/>
+      <c r="C1" s="322"/>
+      <c r="D1" s="322"/>
+      <c r="E1" s="323"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:29" ht="23.25">
-      <c r="A2" s="322" t="s">
+      <c r="A2" s="324" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="323"/>
-      <c r="C2" s="323"/>
-      <c r="D2" s="323"/>
-      <c r="E2" s="324"/>
+      <c r="B2" s="325"/>
+      <c r="C2" s="325"/>
+      <c r="D2" s="325"/>
+      <c r="E2" s="326"/>
       <c r="F2" s="5"/>
       <c r="G2" s="11"/>
       <c r="H2" s="8"/>
@@ -19653,13 +19653,13 @@
       <c r="AC14" s="8"/>
     </row>
     <row r="15" spans="1:29" ht="22.5">
-      <c r="A15" s="325" t="s">
+      <c r="A15" s="327" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="326"/>
-      <c r="C15" s="326"/>
-      <c r="D15" s="326"/>
-      <c r="E15" s="327"/>
+      <c r="B15" s="328"/>
+      <c r="C15" s="328"/>
+      <c r="D15" s="328"/>
+      <c r="E15" s="329"/>
       <c r="F15" s="5"/>
       <c r="G15" s="9"/>
       <c r="H15" s="28"/>

</xml_diff>